<commit_message>
protocols published in previous releases marked with p for guidance
</commit_message>
<xml_diff>
--- a/all_protocols.xlsx
+++ b/all_protocols.xlsx
@@ -20,12 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t xml:space="preserve">Sessions/Subjects</t>
   </si>
   <si>
+    <t xml:space="preserve">First release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second release</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARCHI – screening 3 OLD (3 loc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p</t>
   </si>
   <si>
     <t xml:space="preserve">ARCHI – screening 3 new vs</t>
@@ -182,11 +191,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -207,12 +217,6 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF800000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -286,7 +290,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,19 +304,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,270 +398,314 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A51"/>
+      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
which protocols have videos
</commit_message>
<xml_diff>
--- a/all_protocols.xlsx
+++ b/all_protocols.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t xml:space="preserve">Sessions/Subjects</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">Fifth release</t>
   </si>
   <si>
+    <t xml:space="preserve">Video</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARCHI – screening 3 OLD (3 loc)</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">All ARCHI Localizers</t>
   </si>
   <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
     <t xml:space="preserve">V1</t>
   </si>
   <si>
@@ -103,9 +109,15 @@
     <t xml:space="preserve">Positive-incentive Value</t>
   </si>
   <si>
+    <t xml:space="preserve">preferences?</t>
+  </si>
+  <si>
     <t xml:space="preserve">ToM</t>
   </si>
   <si>
+    <t xml:space="preserve">i </t>
+  </si>
+  <si>
     <t xml:space="preserve">VSTM + Enumeration</t>
   </si>
   <si>
@@ -175,7 +187,7 @@
     <t xml:space="preserve">VS_WM</t>
   </si>
   <si>
-    <t xml:space="preserve">Reward_proc</t>
+    <t xml:space="preserve">Reward_proc + NARPS</t>
   </si>
   <si>
     <t xml:space="preserve">Scene_Face_Body</t>
@@ -410,13 +422,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.11"/>
@@ -445,366 +457,396 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -812,8 +854,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
noting videos that are done
</commit_message>
<xml_diff>
--- a/all_protocols.xlsx
+++ b/all_protocols.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t xml:space="preserve">Sessions/Subjects</t>
   </si>
@@ -424,11 +424,11 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.11"/>
@@ -743,6 +743,9 @@
       <c r="F36" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="G36" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
@@ -783,6 +786,9 @@
       <c r="F41" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="G41" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
@@ -791,6 +797,9 @@
       <c r="F42" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="G42" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
@@ -799,6 +808,9 @@
       <c r="F43" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="G43" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
@@ -806,6 +818,9 @@
       </c>
       <c r="F44" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
small trace for publised videos
</commit_message>
<xml_diff>
--- a/all_protocols.xlsx
+++ b/all_protocols.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
   <si>
     <t xml:space="preserve">Sessions/Subjects</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">Biological Motion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u</t>
   </si>
   <si>
     <t xml:space="preserve">Math-Language protocol</t>
@@ -438,13 +441,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.11"/>
@@ -751,21 +754,24 @@
       <c r="F35" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="G35" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>8</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>8</v>
@@ -773,102 +779,120 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>8</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>8</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>8</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>8</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>8</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>8</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>11</v>
@@ -876,7 +900,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>11</v>
@@ -884,7 +908,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>11</v>
@@ -892,27 +916,27 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>